<commit_message>
up biên bản nghiệm thu
</commit_message>
<xml_diff>
--- a/Mẫu/PTV/thoi gian.xlsx
+++ b/Mẫu/PTV/thoi gian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCKH\Mẫu\PTV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9051A4A-88E5-4B6B-BAF6-6E6922D195B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BC9BCB-955C-4CF0-B36B-99C2BE0A171C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4839FA7E-1DC5-4B04-870C-C7FC1FC75BD7}"/>
   </bookViews>
@@ -30,49 +30,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>3_Em</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>0793303000</t>
   </si>
   <si>
-    <t>3_Nghia</t>
-  </si>
-  <si>
-    <t>4_Khoa</t>
-  </si>
-  <si>
     <t>0334125627</t>
   </si>
   <si>
-    <t>4_Khanh</t>
-  </si>
-  <si>
-    <t>5_Khanh</t>
-  </si>
-  <si>
-    <t>5_Khoa</t>
-  </si>
-  <si>
-    <t>5_Nghia</t>
-  </si>
-  <si>
-    <t>5_Em</t>
+    <t>số ngày</t>
+  </si>
+  <si>
+    <t>tèo</t>
+  </si>
+  <si>
+    <t>khoa</t>
+  </si>
+  <si>
+    <t>bắt đầu</t>
+  </si>
+  <si>
+    <t>nghia</t>
+  </si>
+  <si>
+    <t>cv3:kiểm thử</t>
+  </si>
+  <si>
+    <t>cv3:alumni</t>
+  </si>
+  <si>
+    <t>cv2:admin</t>
+  </si>
+  <si>
+    <t>cv1:thuyết minh</t>
+  </si>
+  <si>
+    <t>cv4:báo cáo</t>
+  </si>
+  <si>
+    <t>(1) Kinh phí đề tài đã thanh toán đến 10/10/2019: 5.430.000 đồng.</t>
+  </si>
+  <si>
+    <t>(2) Khả năng thanh toán đến 31/10/2019: 12.000.000 đồng.</t>
+  </si>
+  <si>
+    <t>(3) Kinh phí không thanh toán được đến 31/12/2019: 0 đồng </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,10 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,148 +436,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D41FE7B-ED30-4056-B99A-6C5FE03E63DD}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
         <v>43587</v>
       </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1">
-        <f>A1+B3</f>
-        <v>43602</v>
-      </c>
-      <c r="D1" s="1">
-        <f>C1+B3</f>
+      <c r="C2" s="1">
+        <f>B2+A7</f>
         <v>43617</v>
       </c>
-      <c r="E1" s="1">
-        <f>D1+B3</f>
-        <v>43632</v>
-      </c>
-      <c r="F1" s="1">
-        <f>E1+B3</f>
-        <v>43647</v>
-      </c>
-      <c r="G1" s="1">
-        <f>F1+B3</f>
+      <c r="D2" s="1">
+        <f>C2+A10</f>
         <v>43662</v>
       </c>
-      <c r="H1" s="1">
-        <f>G1+B4</f>
-        <v>43682</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="E2" s="1">
+        <f>D2+A11</f>
+        <v>43712</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2+A4</f>
+        <v>43727</v>
+      </c>
+      <c r="G2" s="1">
+        <f>F2+A9</f>
+        <v>43767</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="K6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="K7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1">
-        <f>H1+B3</f>
-        <v>43697</v>
-      </c>
-      <c r="J2" s="1">
-        <f>I2+B3</f>
-        <v>43712</v>
-      </c>
-      <c r="K2" s="1">
-        <f>J2+B2</f>
-        <v>43722</v>
-      </c>
-      <c r="L2" s="1">
-        <f>K2+B1</f>
-        <v>43727</v>
-      </c>
-      <c r="M2" s="1">
-        <f>L2+B2</f>
-        <v>43737</v>
-      </c>
-      <c r="N2" s="1">
-        <f>M2+B3</f>
-        <v>43752</v>
-      </c>
-      <c r="O2" s="1">
-        <f>N2+B2</f>
-        <v>43762</v>
-      </c>
-      <c r="P2" s="1">
-        <f>O2+B1</f>
-        <v>43767</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="N3" s="1">
-        <f>L2+B3</f>
-        <v>43742</v>
-      </c>
-      <c r="O3" s="1">
-        <f>L2+B2</f>
-        <v>43737</v>
-      </c>
-      <c r="P3" s="1">
-        <f>L2+B1</f>
-        <v>43732</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D5" s="2" t="s">
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="G15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="G16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="7:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K28"/>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K30"/>
+    </row>
+    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>